<commit_message>
Update salary excel printer result
</commit_message>
<xml_diff>
--- a/HÀ-NOVEMBER-2020.xlsx
+++ b/HÀ-NOVEMBER-2020.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>NAME</t>
   </si>
@@ -24,6 +24,57 @@
   </si>
   <si>
     <t>HOUR</t>
+  </si>
+  <si>
+    <t>MON 02/11</t>
+  </si>
+  <si>
+    <t>13:30 - 17:30</t>
+  </si>
+  <si>
+    <t>WED 04/11</t>
+  </si>
+  <si>
+    <t>FRID 06/11</t>
+  </si>
+  <si>
+    <t>MON 09/11</t>
+  </si>
+  <si>
+    <t>WED 11/11</t>
+  </si>
+  <si>
+    <t>FRID 13/11</t>
+  </si>
+  <si>
+    <t>MON 16/11</t>
+  </si>
+  <si>
+    <t>WED 18/11</t>
+  </si>
+  <si>
+    <t>FRID 20/11</t>
+  </si>
+  <si>
+    <t>MON 23/11</t>
+  </si>
+  <si>
+    <t>WED 25/11</t>
+  </si>
+  <si>
+    <t>FRID 27/11</t>
+  </si>
+  <si>
+    <t>MON 30/11</t>
+  </si>
+  <si>
+    <t>HÀ</t>
+  </si>
+  <si>
+    <t>TOTAL HOUR</t>
+  </si>
+  <si>
+    <t>SALARY</t>
   </si>
 </sst>
 </file>
@@ -31,7 +82,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="61">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -54,6 +105,284 @@
     <font>
       <name val="Times New Roman"/>
       <sz val="14.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="4">
@@ -154,7 +483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyFill="true">
       <alignment horizontal="center"/>
@@ -167,6 +496,174 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyFill="true">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyFill="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyFill="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -180,10 +677,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.0" customHeight="true"/>
   <cols>
-    <col min="2" max="2" width="21.875" customWidth="true"/>
-    <col min="3" max="3" width="21.875" customWidth="true"/>
-    <col min="4" max="4" width="21.875" customWidth="true"/>
-    <col min="5" max="5" width="21.875" customWidth="true"/>
+    <col min="2" max="2" customWidth="true" width="21.875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -200,7 +697,184 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3">
+      <c r="B3" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="45"/>
+      <c r="C4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="10" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="46"/>
+      <c r="C5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="13" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="47"/>
+      <c r="C6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="16" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="48"/>
+      <c r="C7" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="19" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="49"/>
+      <c r="C8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="22" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="50"/>
+      <c r="C9" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="25" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="51"/>
+      <c r="C10" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="28" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="52"/>
+      <c r="C11" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="31" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="53"/>
+      <c r="C12" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="34" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="54"/>
+      <c r="C13" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="37" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="55"/>
+      <c r="C14" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="40" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="56"/>
+      <c r="C15" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="43" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="D16" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="58" t="n">
+        <v>52.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="D17" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="60" t="n">
+        <v>936.0</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells>
+    <mergeCell ref="B3:B15"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>